<commit_message>
book list feature updated
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="24">
   <si>
     <t>Mobile Number</t>
   </si>
@@ -82,6 +82,24 @@
   </si>
   <si>
     <t>SoftSuave114342</t>
+  </si>
+  <si>
+    <t>7980000029</t>
+  </si>
+  <si>
+    <t>test162537</t>
+  </si>
+  <si>
+    <t>test162537@gmail.com</t>
+  </si>
+  <si>
+    <t>SoftSuave121907</t>
+  </si>
+  <si>
+    <t>7980000030</t>
+  </si>
+  <si>
+    <t>7980000031</t>
   </si>
 </sst>
 </file>
@@ -1251,7 +1269,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:D3"/>
@@ -1319,6 +1337,48 @@
       </c>
       <c r="D4" t="s" s="0">
         <v>17</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1577,15 +1637,24 @@
       <c r="A30" s="0">
         <v>7980000029</v>
       </c>
+      <c r="B30" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="0">
         <v>7980000030</v>
       </c>
+      <c r="B31" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="0">
         <v>7980000031</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:1">

</xml_diff>

<commit_message>
allure report and code refactor
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="74">
   <si>
     <t>Mobile Number</t>
   </si>
@@ -100,6 +100,156 @@
   </si>
   <si>
     <t>7980000031</t>
+  </si>
+  <si>
+    <t>7980000033</t>
+  </si>
+  <si>
+    <t>test141236</t>
+  </si>
+  <si>
+    <t>test141236@gmail.com</t>
+  </si>
+  <si>
+    <t>SoftSuave107202</t>
+  </si>
+  <si>
+    <t>7980000037</t>
+  </si>
+  <si>
+    <t>test84456</t>
+  </si>
+  <si>
+    <t>test84456@gmail.com</t>
+  </si>
+  <si>
+    <t>SoftSuave126242</t>
+  </si>
+  <si>
+    <t>7980000038</t>
+  </si>
+  <si>
+    <t>7980000039</t>
+  </si>
+  <si>
+    <t>7980000040</t>
+  </si>
+  <si>
+    <t>test115430</t>
+  </si>
+  <si>
+    <t>test115430@gmail.com</t>
+  </si>
+  <si>
+    <t>SoftSuave18632</t>
+  </si>
+  <si>
+    <t>7980000041</t>
+  </si>
+  <si>
+    <t>7980000042</t>
+  </si>
+  <si>
+    <t>7980000043</t>
+  </si>
+  <si>
+    <t>test77299</t>
+  </si>
+  <si>
+    <t>test77299@gmail.com</t>
+  </si>
+  <si>
+    <t>SoftSuave140913</t>
+  </si>
+  <si>
+    <t>7980000044</t>
+  </si>
+  <si>
+    <t>7980000045</t>
+  </si>
+  <si>
+    <t>7980000046</t>
+  </si>
+  <si>
+    <t>test88162</t>
+  </si>
+  <si>
+    <t>test88162@gmail.com</t>
+  </si>
+  <si>
+    <t>SoftSuave16439</t>
+  </si>
+  <si>
+    <t>7980000047</t>
+  </si>
+  <si>
+    <t>test121329</t>
+  </si>
+  <si>
+    <t>test121329@gmail.com</t>
+  </si>
+  <si>
+    <t>SoftSuave164883</t>
+  </si>
+  <si>
+    <t>7980000048</t>
+  </si>
+  <si>
+    <t>7980000049</t>
+  </si>
+  <si>
+    <t>7980000050</t>
+  </si>
+  <si>
+    <t>test127194</t>
+  </si>
+  <si>
+    <t>test127194@gmail.com</t>
+  </si>
+  <si>
+    <t>SoftSuave107168</t>
+  </si>
+  <si>
+    <t>7980000051</t>
+  </si>
+  <si>
+    <t>7980000052</t>
+  </si>
+  <si>
+    <t>7980000053</t>
+  </si>
+  <si>
+    <t>test59551</t>
+  </si>
+  <si>
+    <t>test59551@gmail.com</t>
+  </si>
+  <si>
+    <t>SoftSuave113390</t>
+  </si>
+  <si>
+    <t>7980000054</t>
+  </si>
+  <si>
+    <t>7980000055</t>
+  </si>
+  <si>
+    <t>7980000056</t>
+  </si>
+  <si>
+    <t>test116858</t>
+  </si>
+  <si>
+    <t>test116858@gmail.com</t>
+  </si>
+  <si>
+    <t>SoftSuave156281</t>
+  </si>
+  <si>
+    <t>7980000057</t>
+  </si>
+  <si>
+    <t>7980000058</t>
   </si>
 </sst>
 </file>
@@ -1269,7 +1419,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:D3"/>
@@ -1379,6 +1529,328 @@
       </c>
       <c r="D7" t="s" s="0">
         <v>21</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s" s="0">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s" s="0">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s" s="0">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="D18" t="s" s="0">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C19" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="D19" t="s" s="0">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="D20" t="s" s="0">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="D21" t="s" s="0">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="D22" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="D23" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="D24" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="D25" t="s" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="C26" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="D26" t="s" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="D27" t="s" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="D28" t="s" s="0">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="D29" t="s" s="0">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="D30" t="s" s="0">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1661,135 +2133,216 @@
       <c r="A33" s="0">
         <v>7980000032</v>
       </c>
+      <c r="B33" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="0">
         <v>7980000033</v>
       </c>
+      <c r="B34" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="0">
         <v>7980000034</v>
       </c>
+      <c r="B35" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="0">
         <v>7980000035</v>
       </c>
+      <c r="B36" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="0">
         <v>7980000036</v>
       </c>
+      <c r="B37" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="0">
         <v>7980000037</v>
       </c>
+      <c r="B38" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="0">
         <v>7980000038</v>
       </c>
+      <c r="B39" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="0">
         <v>7980000039</v>
       </c>
+      <c r="B40" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="0">
         <v>7980000040</v>
       </c>
+      <c r="B41" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="0">
         <v>7980000041</v>
       </c>
+      <c r="B42" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="0">
         <v>7980000042</v>
       </c>
+      <c r="B43" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="0">
         <v>7980000043</v>
       </c>
+      <c r="B44" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="0">
         <v>7980000044</v>
       </c>
+      <c r="B45" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="0">
         <v>7980000045</v>
       </c>
+      <c r="B46" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="0">
         <v>7980000046</v>
       </c>
+      <c r="B47" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="0">
         <v>7980000047</v>
       </c>
+      <c r="B48" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="0">
         <v>7980000048</v>
       </c>
+      <c r="B49" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="0">
         <v>7980000049</v>
       </c>
+      <c r="B50" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="0">
         <v>7980000050</v>
       </c>
+      <c r="B51" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="0">
         <v>7980000051</v>
       </c>
+      <c r="B52" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="0">
         <v>7980000052</v>
       </c>
+      <c r="B53" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="0">
         <v>7980000053</v>
       </c>
+      <c r="B54" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="0">
         <v>7980000054</v>
       </c>
+      <c r="B55" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="0">
         <v>7980000055</v>
       </c>
+      <c r="B56" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="0">
         <v>7980000056</v>
       </c>
+      <c r="B57" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="0">
         <v>7980000057</v>
       </c>
+      <c r="B58" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="0">
         <v>7980000058</v>
+      </c>
+      <c r="B59" t="s" s="0">
+        <v>13</v>
       </c>
     </row>
     <row r="60" spans="1:1">

</xml_diff>

<commit_message>
added material entry scenarios
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="84">
   <si>
     <t>Mobile Number</t>
   </si>
@@ -250,6 +250,36 @@
   </si>
   <si>
     <t>7980000058</t>
+  </si>
+  <si>
+    <t>7980000059</t>
+  </si>
+  <si>
+    <t>test10030</t>
+  </si>
+  <si>
+    <t>test10030@gmail.com</t>
+  </si>
+  <si>
+    <t>SoftSuave21420</t>
+  </si>
+  <si>
+    <t>7980000060</t>
+  </si>
+  <si>
+    <t>7980000061</t>
+  </si>
+  <si>
+    <t>7980000062</t>
+  </si>
+  <si>
+    <t>7980000063</t>
+  </si>
+  <si>
+    <t>7980000064</t>
+  </si>
+  <si>
+    <t>7980000065</t>
   </si>
 </sst>
 </file>
@@ -1419,7 +1449,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:D3"/>
@@ -1851,6 +1881,104 @@
       </c>
       <c r="D30" t="s" s="0">
         <v>71</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="C31" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="D31" t="s" s="0">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="C32" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="D32" t="s" s="0">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="C33" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="D33" t="s" s="0">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="C34" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="D34" t="s" s="0">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="C35" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="D35" t="s" s="0">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="B36" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="C36" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="D36" t="s" s="0">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="B37" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="C37" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="D37" t="s" s="0">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2349,35 +2477,56 @@
       <c r="A60" s="0">
         <v>7980000059</v>
       </c>
+      <c r="B60" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="0">
         <v>7980000060</v>
       </c>
+      <c r="B61" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="0">
         <v>7980000061</v>
       </c>
+      <c r="B62" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" s="0">
         <v>7980000062</v>
       </c>
+      <c r="B63" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="0">
         <v>7980000063</v>
       </c>
+      <c r="B64" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="0">
         <v>7980000064</v>
       </c>
+      <c r="B65" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="0">
         <v>7980000065</v>
+      </c>
+      <c r="B66" t="s" s="0">
+        <v>13</v>
       </c>
     </row>
     <row r="67" spans="1:1">

</xml_diff>

<commit_message>
added failure screenshot fucntionality in allure report
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="90">
   <si>
     <t>Mobile Number</t>
   </si>
@@ -280,6 +280,24 @@
   </si>
   <si>
     <t>7980000065</t>
+  </si>
+  <si>
+    <t>7980000066</t>
+  </si>
+  <si>
+    <t>test151776</t>
+  </si>
+  <si>
+    <t>test151776@gmail.com</t>
+  </si>
+  <si>
+    <t>SoftSuave52224</t>
+  </si>
+  <si>
+    <t>7980000067</t>
+  </si>
+  <si>
+    <t>7980000068</t>
   </si>
 </sst>
 </file>
@@ -1449,7 +1467,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:D3"/>
@@ -1979,6 +1997,48 @@
       </c>
       <c r="D37" t="s" s="0">
         <v>77</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="B38" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="C38" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="D38" t="s" s="0">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B39" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="C39" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="D39" t="s" s="0">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="B40" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="C40" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="D40" t="s" s="0">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2533,15 +2593,24 @@
       <c r="A67" s="0">
         <v>7980000066</v>
       </c>
+      <c r="B67" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="0">
         <v>7980000067</v>
       </c>
+      <c r="B68" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="0">
         <v>7980000068</v>
+      </c>
+      <c r="B69" t="s" s="0">
+        <v>13</v>
       </c>
     </row>
     <row r="70" spans="1:1">

</xml_diff>

<commit_message>
all scenarios run successfully
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="114">
   <si>
     <t>Mobile Number</t>
   </si>
@@ -298,6 +298,78 @@
   </si>
   <si>
     <t>7980000068</t>
+  </si>
+  <si>
+    <t>7980000069</t>
+  </si>
+  <si>
+    <t>test68629</t>
+  </si>
+  <si>
+    <t>test68629@gmail.com</t>
+  </si>
+  <si>
+    <t>SoftSuave6273</t>
+  </si>
+  <si>
+    <t>7980000070</t>
+  </si>
+  <si>
+    <t>7980000072</t>
+  </si>
+  <si>
+    <t>7980000073</t>
+  </si>
+  <si>
+    <t>test44642</t>
+  </si>
+  <si>
+    <t>test44642@gmail.com</t>
+  </si>
+  <si>
+    <t>SoftSuave101694</t>
+  </si>
+  <si>
+    <t>7980000074</t>
+  </si>
+  <si>
+    <t>7980000075</t>
+  </si>
+  <si>
+    <t>7980000076</t>
+  </si>
+  <si>
+    <t>test86530</t>
+  </si>
+  <si>
+    <t>test86530@gmail.com</t>
+  </si>
+  <si>
+    <t>SoftSuave105706</t>
+  </si>
+  <si>
+    <t>7980000077</t>
+  </si>
+  <si>
+    <t>7980000078</t>
+  </si>
+  <si>
+    <t>7980000079</t>
+  </si>
+  <si>
+    <t>test14552</t>
+  </si>
+  <si>
+    <t>test14552@gmail.com</t>
+  </si>
+  <si>
+    <t>SoftSuave148393</t>
+  </si>
+  <si>
+    <t>7980000080</t>
+  </si>
+  <si>
+    <t>7980000081</t>
   </si>
 </sst>
 </file>
@@ -1467,7 +1539,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:D3"/>
@@ -2039,6 +2111,174 @@
       </c>
       <c r="D40" t="s" s="0">
         <v>87</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="B41" t="s" s="0">
+        <v>91</v>
+      </c>
+      <c r="C41" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="D41" t="s" s="0">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>91</v>
+      </c>
+      <c r="C42" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="D42" t="s" s="0">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>91</v>
+      </c>
+      <c r="C43" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="D43" t="s" s="0">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>97</v>
+      </c>
+      <c r="C44" t="s" s="0">
+        <v>98</v>
+      </c>
+      <c r="D44" t="s" s="0">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>97</v>
+      </c>
+      <c r="C45" t="s" s="0">
+        <v>98</v>
+      </c>
+      <c r="D45" t="s" s="0">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>101</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>97</v>
+      </c>
+      <c r="C46" t="s" s="0">
+        <v>98</v>
+      </c>
+      <c r="D46" t="s" s="0">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>103</v>
+      </c>
+      <c r="C47" t="s" s="0">
+        <v>104</v>
+      </c>
+      <c r="D47" t="s" s="0">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>103</v>
+      </c>
+      <c r="C48" t="s" s="0">
+        <v>104</v>
+      </c>
+      <c r="D48" t="s" s="0">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>107</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>103</v>
+      </c>
+      <c r="C49" t="s" s="0">
+        <v>104</v>
+      </c>
+      <c r="D49" t="s" s="0">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>108</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="C50" t="s" s="0">
+        <v>110</v>
+      </c>
+      <c r="D50" t="s" s="0">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="B51" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="C51" t="s" s="0">
+        <v>110</v>
+      </c>
+      <c r="D51" t="s" s="0">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="B52" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="C52" t="s" s="0">
+        <v>110</v>
+      </c>
+      <c r="D52" t="s" s="0">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2617,65 +2857,104 @@
       <c r="A70" s="0">
         <v>7980000069</v>
       </c>
+      <c r="B70" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="0">
         <v>7980000070</v>
       </c>
+      <c r="B71" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="0">
         <v>7980000071</v>
       </c>
+      <c r="B72" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="0">
         <v>7980000072</v>
       </c>
+      <c r="B73" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" s="0">
         <v>7980000073</v>
       </c>
+      <c r="B74" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" s="0">
         <v>7980000074</v>
       </c>
+      <c r="B75" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="0">
         <v>7980000075</v>
       </c>
+      <c r="B76" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" s="0">
         <v>7980000076</v>
       </c>
+      <c r="B77" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" s="0">
         <v>7980000077</v>
       </c>
+      <c r="B78" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" s="0">
         <v>7980000078</v>
       </c>
+      <c r="B79" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" s="0">
         <v>7980000079</v>
       </c>
+      <c r="B80" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" s="0">
         <v>7980000080</v>
       </c>
+      <c r="B81" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" s="0">
         <v>7980000081</v>
+      </c>
+      <c r="B82" t="s" s="0">
+        <v>13</v>
       </c>
     </row>
     <row r="83" spans="1:1">

</xml_diff>